<commit_message>
Add and process raw data
</commit_message>
<xml_diff>
--- a/inst/extdata/dowaodf.xlsx
+++ b/inst/extdata/dowaodf.xlsx
@@ -14,106 +14,106 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
   <si>
-    <t xml:space="preserve">Date survey was completed</t>
+    <t xml:space="preserve">survey_date</t>
   </si>
   <si>
-    <t xml:space="preserve">District</t>
+    <t xml:space="preserve">district</t>
   </si>
   <si>
-    <t xml:space="preserve">GVH</t>
+    <t xml:space="preserve">gvh</t>
   </si>
   <si>
-    <t xml:space="preserve">Health Facility</t>
+    <t xml:space="preserve">health_facility</t>
   </si>
   <si>
-    <t xml:space="preserve">Have you observed a sanitation facility at this household?</t>
+    <t xml:space="preserve">sanitation_observed</t>
   </si>
   <si>
-    <t xml:space="preserve">What type of sanitation facility is it?</t>
+    <t xml:space="preserve">sanitation_type</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this sanitation facility have a pit cover or a water seal (preventing flies from entering the pit)?</t>
+    <t xml:space="preserve">pit_cover_or_seal</t>
   </si>
   <si>
-    <t xml:space="preserve">Is this sanitation facility located within 30m or less away from a water point?</t>
+    <t xml:space="preserve">sanitation_near_water</t>
   </si>
   <si>
-    <t xml:space="preserve">How far is the sanitation facility from the household?</t>
+    <t xml:space="preserve">sanitation_distance</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this sanitation facility offer privacy?</t>
+    <t xml:space="preserve">has_privacy</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this sanitation facility offer security?</t>
+    <t xml:space="preserve">has_security</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this sanitation facility have a roof (preventing rain from coming in)?</t>
+    <t xml:space="preserve">has_roof</t>
   </si>
   <si>
-    <t xml:space="preserve">Is this sanitation facility shared with other household(s)</t>
+    <t xml:space="preserve">shared_sanitation</t>
   </si>
   <si>
-    <t xml:space="preserve">If you have any children, where do you dispose of their faeces?</t>
+    <t xml:space="preserve">child_faeces_disposal</t>
   </si>
   <si>
-    <t xml:space="preserve">If you have any children, where do you dispose of their faeces? (Other) - specify</t>
+    <t xml:space="preserve">child_faeces_disposal_other</t>
   </si>
   <si>
-    <t xml:space="preserve">Where do household members normally defecate?</t>
+    <t xml:space="preserve">usual_defecation_place</t>
   </si>
   <si>
-    <t xml:space="preserve">Have you or any member of your family recently seen/observed faeces in the bushes, field or anywhere lying around in this village (in the past 6 months?)</t>
+    <t xml:space="preserve">faeces_seen_in_village</t>
   </si>
   <si>
-    <t xml:space="preserve">Are there any faeces observable around this household?</t>
+    <t xml:space="preserve">faeces_around_house</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there a hand washing facility within 10 paces away from this sanitation facility?</t>
+    <t xml:space="preserve">handwash_near_sanitation</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there water available at this hand washing facility?</t>
+    <t xml:space="preserve">handwash_has_water</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there soap provided at this hand washing facility?</t>
+    <t xml:space="preserve">handwash_has_soap</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there evidence that the hand washing facility is being used?</t>
+    <t xml:space="preserve">handwash_in_use</t>
   </si>
   <si>
-    <t xml:space="preserve">Which type of materials are used by women in this household to collect/absorb menstrual blood?</t>
+    <t xml:space="preserve">mhm_materials_used</t>
   </si>
   <si>
-    <t xml:space="preserve">If the MHM are reusable, are these cleaned?</t>
+    <t xml:space="preserve">mhm_cleaned</t>
   </si>
   <si>
-    <t xml:space="preserve">How are these cleaned?</t>
+    <t xml:space="preserve">mhm_cleaning_method</t>
   </si>
   <si>
-    <t xml:space="preserve">How are the MHM materials dried?</t>
+    <t xml:space="preserve">mhm_drying_method</t>
   </si>
   <si>
-    <t xml:space="preserve">Where are the MHM materials disposed?</t>
+    <t xml:space="preserve">mhm_disposal_place</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this household have a bathroom facility?</t>
+    <t xml:space="preserve">has_bathroom</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there sufficient water available for bathing?</t>
+    <t xml:space="preserve">bathing_has_water</t>
   </si>
   <si>
-    <t xml:space="preserve">What is the water source?</t>
+    <t xml:space="preserve">bathing_water_source</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this bathroom facility have available soap?</t>
+    <t xml:space="preserve">bathroom_has_soap</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there evidence that the bath facility is being used?</t>
+    <t xml:space="preserve">bathroom_in_use</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this bathroom offer privacy?</t>
+    <t xml:space="preserve">bathroom_has_privacy</t>
   </si>
   <si>
-    <t xml:space="preserve">Does this bathroom offer security?</t>
+    <t xml:space="preserve">bathroom_has_security</t>
   </si>
   <si>
     <t xml:space="preserve">7/1/2019</t>

</xml_diff>